<commit_message>
updated results with 2 X 1 billion runs
</commit_message>
<xml_diff>
--- a/20 Results/meanRate.xlsx
+++ b/20 Results/meanRate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>NSP1</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Substitutions/Site/Year</t>
+  </si>
+  <si>
+    <t>combined data from 2 X 1 billion runs</t>
   </si>
 </sst>
 </file>
@@ -243,9 +246,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -260,30 +263,36 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>NSP5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VP1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$F$10</c:f>
+              <c:f>Sheet1!$B$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.8133999999999999E-3</c:v>
+                  <c:v>7.8062000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1414999999999999E-3</c:v>
+                  <c:v>1.1597999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1304000000000002E-3</c:v>
+                  <c:v>3.1148999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3699999999999999E-2</c:v>
+                  <c:v>2.3400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0122999999999999E-3</c:v>
+                  <c:v>2.0144999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5189000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,9 +342,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -350,30 +359,36 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>NSP5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VP1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$F$11</c:f>
+              <c:f>Sheet1!$B$11:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.411E-3</c:v>
+                  <c:v>4.398E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3010000000000004E-4</c:v>
+                  <c:v>5.329E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6980000000000001E-3</c:v>
+                  <c:v>1.6969999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6039999999999999E-2</c:v>
+                  <c:v>1.601E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0549999999999999E-3</c:v>
+                  <c:v>1.0560000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.263E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,9 +438,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -440,30 +455,36 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>NSP5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VP1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.6383000000000001E-3</c:v>
+                  <c:v>1.6259E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3176999999999993E-5</c:v>
+                  <c:v>9.2380999999999995E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9130999999999995E-4</c:v>
+                  <c:v>5.8540999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.044E-3</c:v>
+                  <c:v>8.9482999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7924999999999998E-4</c:v>
+                  <c:v>2.8048999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7149999999999996E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1705,13 +1726,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1728,8 +1749,10 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1797,21 +1820,23 @@
         <v>12</v>
       </c>
       <c r="B10" s="3">
-        <v>7.8133999999999999E-3</v>
+        <v>7.8062000000000001E-3</v>
       </c>
       <c r="C10" s="3">
-        <v>1.1414999999999999E-3</v>
+        <v>1.1597999999999999E-3</v>
       </c>
       <c r="D10" s="4">
-        <v>3.1304000000000002E-3</v>
+        <v>3.1148999999999999E-3</v>
       </c>
       <c r="E10" s="4">
-        <v>2.3699999999999999E-2</v>
+        <v>2.3400000000000001E-2</v>
       </c>
       <c r="F10" s="4">
-        <v>2.0122999999999999E-3</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>2.0144999999999998E-3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2.5189000000000001E-3</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1823,19 +1848,22 @@
         <v>13</v>
       </c>
       <c r="B11" s="4">
-        <v>4.411E-3</v>
+        <v>4.398E-3</v>
       </c>
       <c r="C11" s="4">
-        <v>5.3010000000000004E-4</v>
+        <v>5.329E-4</v>
       </c>
       <c r="D11" s="3">
-        <v>1.6980000000000001E-3</v>
+        <v>1.6969999999999999E-3</v>
       </c>
       <c r="E11" s="3">
-        <v>1.6039999999999999E-2</v>
+        <v>1.601E-2</v>
       </c>
       <c r="F11" s="3">
-        <v>1.0549999999999999E-3</v>
+        <v>1.0560000000000001E-3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.263E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1843,19 +1871,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>1.6383000000000001E-3</v>
+        <v>1.6259E-3</v>
       </c>
       <c r="C12" s="3">
-        <v>8.3176999999999993E-5</v>
+        <v>9.2380999999999995E-5</v>
       </c>
       <c r="D12" s="3">
-        <v>5.9130999999999995E-4</v>
+        <v>5.8540999999999997E-4</v>
       </c>
       <c r="E12" s="3">
-        <v>9.044E-3</v>
+        <v>8.9482999999999993E-3</v>
       </c>
       <c r="F12" s="3">
-        <v>2.7924999999999998E-4</v>
+        <v>2.8048999999999999E-4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5.7149999999999996E-4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed an duplication error in VP6A sequence set for post vaccine analysis
</commit_message>
<xml_diff>
--- a/20 Results/meanRate.xlsx
+++ b/20 Results/meanRate.xlsx
@@ -246,9 +246,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$9:$I$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -266,16 +266,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>VP1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VP2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VP3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>7.8062000000000001E-3</c:v>
                 </c:pt>
@@ -293,6 +299,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.5189000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.3981000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9502E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -342,9 +354,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$9:$I$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -362,16 +374,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>VP1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VP2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VP3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$G$11</c:f>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>4.398E-3</c:v>
                 </c:pt>
@@ -389,6 +407,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.263E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4729999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6199999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,9 +462,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$9:$I$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -458,16 +482,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>VP1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VP2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VP3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$G$12</c:f>
+              <c:f>Sheet1!$B$12:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.6259E-3</c:v>
                 </c:pt>
@@ -485,6 +515,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.7149999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.7131999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5035999999999996E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1726,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,8 +1873,12 @@
       <c r="G10" s="4">
         <v>2.5189000000000001E-3</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="H10" s="4">
+        <v>4.3981000000000003E-3</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2.9502E-3</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1865,6 +1905,12 @@
       <c r="G11" s="3">
         <v>1.263E-3</v>
       </c>
+      <c r="H11" s="3">
+        <v>2.4729999999999999E-3</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.6199999999999999E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1887,6 +1933,12 @@
       </c>
       <c r="G12" s="3">
         <v>5.7149999999999996E-4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>8.7131999999999997E-4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>5.5035999999999996E-4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated meanrate for RVB
</commit_message>
<xml_diff>
--- a/20 Results/meanRate.xlsx
+++ b/20 Results/meanRate.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RVC" sheetId="1" r:id="rId1"/>
+    <sheet name="RVB" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>NSP1</t>
   </si>
@@ -213,7 +214,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>RVC!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -246,7 +247,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$I$9</c:f>
+              <c:f>RVC!$B$9:$I$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -278,7 +279,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:f>RVC!$B$10:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -321,7 +322,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>RVC!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -354,7 +355,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$I$9</c:f>
+              <c:f>RVC!$B$9:$I$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -386,7 +387,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:f>RVC!$B$11:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -429,7 +430,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>RVC!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -462,7 +463,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$I$9</c:f>
+              <c:f>RVC!$B$9:$I$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -494,7 +495,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$I$12</c:f>
+              <c:f>RVC!$B$12:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -529,6 +530,765 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0833-4893-9D63-15B54EF98E4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:axId val="313618336"/>
+        <c:axId val="313618664"/>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="313618336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Proteins</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="313618664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="313618664"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Substitutions/Site/Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="313618336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Estimated Mutation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-SG" baseline="0"/>
+              <a:t> Rates of Different Proteins</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RVB!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Upper 95% HPD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>RVB!$B$9:$J$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>NSP1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NSP2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NSP3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NSP4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NSP5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VP1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VP2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VP3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VP4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>RVB!$B$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.01E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7412999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5370000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.77E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9718000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0533000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0BED-4C21-9D24-DC5C1D8052A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RVB!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Substitutions/Site/Year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>RVB!$B$9:$J$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>NSP1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NSP2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NSP3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NSP4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NSP5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VP1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VP2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VP3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VP4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>RVB!$B$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.539E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8240000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8046999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4450000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.23E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5509999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.7130000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9180000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9099999999999998E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0BED-4C21-9D24-DC5C1D8052A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RVB!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower 95% HPD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>RVB!$B$9:$J$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>NSP1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NSP2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NSP3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NSP4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NSP5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VP1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VP2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VP3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VP4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>RVB!$B$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.5972999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8526000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3802E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8612999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6161000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3535999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2378999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8228000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -912,7 +1672,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1447,6 +2763,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1762,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,4 +3322,225 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9.01E-2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3.7412999999999999E-3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4.5370000000000002E-3</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8.77E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.9718000000000002E-3</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="J10" s="4">
+        <v>4.0533000000000001E-3</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4.539E-2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.8240000000000001E-3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.8046999999999998E-3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.4450000000000003E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.23E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2.5509999999999999E-3</v>
+      </c>
+      <c r="H11" s="3">
+        <v>8.7130000000000003E-3</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.9180000000000001E-2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2.9099999999999998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>9.5972999999999996E-3</v>
+      </c>
+      <c r="C12" s="3">
+        <v>6.8526000000000004E-4</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.3802E-3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5.8612999999999998E-3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.6161000000000001E-3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.3535999999999999E-3</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.2378999999999999E-3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.8228000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added some meanRate results, MEME reports and IQtree files
</commit_message>
<xml_diff>
--- a/20 Results/meanRate.xlsx
+++ b/20 Results/meanRate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="RVA" sheetId="4" r:id="rId1"/>
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -124,9 +124,10 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,8 +325,14 @@
                 <c:pt idx="6">
                   <c:v>2.6738E-3</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0722000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4900999999999999E-3</c:v>
+                </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9113999999999999E-3</c:v>
+                  <c:v>1.9476000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2.7199999999999998E-2</c:v>
@@ -441,8 +448,14 @@
                 <c:pt idx="6">
                   <c:v>1.9653000000000001E-3</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.421E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.317E-3</c:v>
+                </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1869999999999999E-3</c:v>
+                  <c:v>1.1980000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.17E-2</c:v>
@@ -558,8 +571,14 @@
                 <c:pt idx="6">
                   <c:v>1.2939E-3</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.989E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3142E-3</c:v>
+                </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.3713000000000003E-4</c:v>
+                  <c:v>5.4595999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9.4693999999999995E-6</c:v>
@@ -596,11 +615,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="387525760"/>
-        <c:axId val="387512880"/>
+        <c:axId val="264848064"/>
+        <c:axId val="264848624"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="387525760"/>
+        <c:axId val="264848064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +718,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387512880"/>
+        <c:crossAx val="264848624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -708,7 +727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="387512880"/>
+        <c:axId val="264848624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -836,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387525760"/>
+        <c:crossAx val="264848064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1002,9 +1021,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>RVB!$B$9:$J$9</c:f>
+              <c:f>RVB!$B$9:$L$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -1031,16 +1050,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>VP4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>VP6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>VP7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RVB!$B$10:$J$10</c:f>
+              <c:f>RVB!$B$10:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>9.01E-2</c:v>
                 </c:pt>
@@ -1067,6 +1092,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4.0533000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3138E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3947000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1116,9 +1147,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>RVB!$B$9:$J$9</c:f>
+              <c:f>RVB!$B$9:$L$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -1145,16 +1176,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>VP4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>VP6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>VP7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RVB!$B$11:$J$11</c:f>
+              <c:f>RVB!$B$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>4.539E-2</c:v>
                 </c:pt>
@@ -1181,6 +1218,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.9099999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2620000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.212E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1230,9 +1273,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>RVB!$B$9:$J$9</c:f>
+              <c:f>RVB!$B$9:$L$9</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -1259,16 +1302,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>VP4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>VP6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>VP7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RVB!$B$12:$J$12</c:f>
+              <c:f>RVB!$B$12:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>9.5972999999999996E-3</c:v>
                 </c:pt>
@@ -1295,6 +1344,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.8228000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2882E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1594000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,11 +1383,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="381364832"/>
-        <c:axId val="381363152"/>
+        <c:axId val="264852544"/>
+        <c:axId val="264853104"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="381364832"/>
+        <c:axId val="264852544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381363152"/>
+        <c:crossAx val="264853104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1440,7 +1495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381363152"/>
+        <c:axId val="264853104"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1568,7 +1623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381364832"/>
+        <c:crossAx val="264852544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1734,9 +1789,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>RVC!$B$9:$I$9</c:f>
+              <c:f>RVC!$B$9:$L$9</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -1760,16 +1815,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>VP3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VP4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>VP6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>VP7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RVC!$B$10:$I$10</c:f>
+              <c:f>RVC!$B$10:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>7.8062000000000001E-3</c:v>
                 </c:pt>
@@ -1793,6 +1857,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.9502E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1016000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1842,9 +1909,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>RVC!$B$9:$I$9</c:f>
+              <c:f>RVC!$B$9:$L$9</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -1868,16 +1935,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>VP3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VP4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>VP6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>VP7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RVC!$B$11:$I$11</c:f>
+              <c:f>RVC!$B$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>4.398E-3</c:v>
                 </c:pt>
@@ -1901,6 +1977,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.6199999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8620000000000003E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1950,9 +2029,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>RVC!$B$9:$I$9</c:f>
+              <c:f>RVC!$B$9:$L$9</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>NSP1</c:v>
                 </c:pt>
@@ -1976,16 +2055,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>VP3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VP4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>VP6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>VP7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RVC!$B$12:$I$12</c:f>
+              <c:f>RVC!$B$12:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.6259E-3</c:v>
                 </c:pt>
@@ -2009,6 +2097,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5.5035999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.7538000000000002E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2042,11 +2133,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="381366512"/>
-        <c:axId val="381369312"/>
+        <c:axId val="264857024"/>
+        <c:axId val="264857584"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="381366512"/>
+        <c:axId val="264857024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,7 +2236,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381369312"/>
+        <c:crossAx val="264857584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2154,7 +2245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381369312"/>
+        <c:axId val="264857584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2282,7 +2373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381366512"/>
+        <c:crossAx val="264857024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3077,11 +3168,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="477045904"/>
-        <c:axId val="477046464"/>
+        <c:axId val="384218144"/>
+        <c:axId val="384218704"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="477045904"/>
+        <c:axId val="384218144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3194,7 +3285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477046464"/>
+        <c:crossAx val="384218704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3203,7 +3294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477046464"/>
+        <c:axId val="384218704"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3331,7 +3422,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477045904"/>
+        <c:crossAx val="384218144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3546,7 +3637,7 @@
                   <c:v>4.3981000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.0722000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5.9400000000000001E-2</c:v>
@@ -3555,19 +3646,19 @@
                   <c:v>2.9502E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.4900999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4.0533000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.1016000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9113999999999999E-3</c:v>
+                  <c:v>1.9476000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.3138E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1E-3</c:v>
@@ -3576,7 +3667,7 @@
                   <c:v>2.7199999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.3947000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1E-3</c:v>
@@ -4020,7 +4111,7 @@
                   <c:v>2.4729999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.421E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.9180000000000001E-2</c:v>
@@ -4029,19 +4120,19 @@
                   <c:v>1.6199999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.317E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2.9099999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1E-3</c:v>
+                  <c:v>7.8620000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1869999999999999E-3</c:v>
+                  <c:v>1.1980000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.2620000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1E-3</c:v>
@@ -4050,7 +4141,7 @@
                   <c:v>1.17E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.212E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1E-3</c:v>
@@ -4152,7 +4243,7 @@
                   <c:v>8.7131999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1E-3</c:v>
+                  <c:v>8.989E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.2378999999999999E-3</c:v>
@@ -4161,19 +4252,19 @@
                   <c:v>5.5035999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.3142E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.8228000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1E-3</c:v>
+                  <c:v>4.7538000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.3713000000000003E-4</c:v>
+                  <c:v>5.4595999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.2882E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1E-3</c:v>
@@ -4182,7 +4273,7 @@
                   <c:v>9.4693999999999995E-6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.1594000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1E-3</c:v>
@@ -4219,11 +4310,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="471050704"/>
-        <c:axId val="471055184"/>
+        <c:axId val="384222624"/>
+        <c:axId val="384223184"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="471050704"/>
+        <c:axId val="384222624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4336,7 +4427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471055184"/>
+        <c:crossAx val="384223184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4345,7 +4436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471055184"/>
+        <c:axId val="384223184"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4473,7 +4564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471050704"/>
+        <c:crossAx val="384222624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7784,8 +7875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7866,7 +7957,7 @@
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="L9" t="s">
@@ -7896,10 +7987,14 @@
       <c r="H10" s="4">
         <v>2.6738E-3</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6">
-        <v>1.9113999999999999E-3</v>
+      <c r="I10" s="4">
+        <v>2.0722000000000002E-3</v>
+      </c>
+      <c r="J10" s="4">
+        <v>3.4900999999999999E-3</v>
+      </c>
+      <c r="K10" s="7">
+        <v>1.9476000000000001E-3</v>
       </c>
       <c r="L10" s="4">
         <v>2.7199999999999998E-2</v>
@@ -7927,8 +8022,14 @@
       <c r="H11" s="3">
         <v>1.9653000000000001E-3</v>
       </c>
-      <c r="K11" s="7">
-        <v>1.1869999999999999E-3</v>
+      <c r="I11" s="3">
+        <v>1.421E-3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2.317E-3</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1.1980000000000001E-3</v>
       </c>
       <c r="L11" s="3">
         <v>1.17E-2</v>
@@ -7957,10 +8058,14 @@
       <c r="H12" s="3">
         <v>1.2939E-3</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="7">
-        <v>5.3713000000000003E-4</v>
+      <c r="I12" s="3">
+        <v>8.989E-4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.3142E-3</v>
+      </c>
+      <c r="K12" s="8">
+        <v>5.4595999999999996E-4</v>
       </c>
       <c r="L12" s="3">
         <v>9.4693999999999995E-6</v>
@@ -8000,8 +8105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J12"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8120,8 +8225,12 @@
       <c r="J10" s="4">
         <v>4.0533000000000001E-3</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="K10" s="4">
+        <v>3.3138E-3</v>
+      </c>
+      <c r="L10" s="4">
+        <v>3.3947000000000001E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -8154,6 +8263,12 @@
       <c r="J11" s="3">
         <v>2.9099999999999998E-3</v>
       </c>
+      <c r="K11" s="3">
+        <v>2.2620000000000001E-3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2.212E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -8185,6 +8300,12 @@
       </c>
       <c r="J12" s="3">
         <v>1.8228000000000001E-3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.2882E-3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1.1594000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -8222,7 +8343,7 @@
   <dimension ref="A6:L15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I12"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8338,7 +8459,9 @@
       <c r="I10" s="4">
         <v>2.9502E-3</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4">
+        <v>1.1016000000000001E-3</v>
+      </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
@@ -8370,6 +8493,9 @@
       <c r="I11" s="3">
         <v>1.6199999999999999E-3</v>
       </c>
+      <c r="J11" s="3">
+        <v>7.8620000000000003E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -8398,6 +8524,9 @@
       </c>
       <c r="I12" s="3">
         <v>5.5035999999999996E-4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>4.7538000000000002E-4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -8777,8 +8906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8899,7 +9028,7 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>1E-3</v>
       </c>
       <c r="C10" s="4">
@@ -8917,8 +9046,8 @@
       <c r="G10" s="4">
         <v>4.3981000000000003E-3</v>
       </c>
-      <c r="H10" s="7">
-        <v>1E-3</v>
+      <c r="H10" s="4">
+        <v>2.0722000000000002E-3</v>
       </c>
       <c r="I10" s="4">
         <v>5.9400000000000001E-2</v>
@@ -8926,31 +9055,31 @@
       <c r="J10" s="4">
         <v>2.9502E-3</v>
       </c>
-      <c r="K10" s="7">
-        <v>1E-3</v>
+      <c r="K10" s="4">
+        <v>3.4900999999999999E-3</v>
       </c>
       <c r="L10" s="4">
         <v>4.0533000000000001E-3</v>
       </c>
-      <c r="M10" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="N10" s="6">
-        <v>1.9113999999999999E-3</v>
-      </c>
-      <c r="O10" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="P10" s="7">
+      <c r="M10" s="4">
+        <v>1.1016000000000001E-3</v>
+      </c>
+      <c r="N10" s="7">
+        <v>1.9476000000000001E-3</v>
+      </c>
+      <c r="O10" s="4">
+        <v>3.3138E-3</v>
+      </c>
+      <c r="P10" s="5">
         <v>1E-3</v>
       </c>
       <c r="Q10" s="4">
         <v>2.7199999999999998E-2</v>
       </c>
-      <c r="R10" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S10" s="7">
+      <c r="R10" s="4">
+        <v>3.3947000000000001E-3</v>
+      </c>
+      <c r="S10" s="5">
         <v>1E-3</v>
       </c>
       <c r="U10" s="4"/>
@@ -8960,7 +9089,7 @@
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>1E-3</v>
       </c>
       <c r="C11" s="3">
@@ -8978,8 +9107,8 @@
       <c r="G11" s="3">
         <v>2.4729999999999999E-3</v>
       </c>
-      <c r="H11" s="7">
-        <v>1E-3</v>
+      <c r="H11" s="3">
+        <v>1.421E-3</v>
       </c>
       <c r="I11" s="3">
         <v>2.9180000000000001E-2</v>
@@ -8987,31 +9116,31 @@
       <c r="J11" s="3">
         <v>1.6199999999999999E-3</v>
       </c>
-      <c r="K11" s="7">
-        <v>1E-3</v>
+      <c r="K11" s="3">
+        <v>2.317E-3</v>
       </c>
       <c r="L11" s="3">
         <v>2.9099999999999998E-3</v>
       </c>
-      <c r="M11" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="N11" s="7">
-        <v>1.1869999999999999E-3</v>
-      </c>
-      <c r="O11" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="P11" s="7">
+      <c r="M11" s="3">
+        <v>7.8620000000000003E-4</v>
+      </c>
+      <c r="N11" s="8">
+        <v>1.1980000000000001E-3</v>
+      </c>
+      <c r="O11" s="3">
+        <v>2.2620000000000001E-3</v>
+      </c>
+      <c r="P11" s="5">
         <v>1E-3</v>
       </c>
       <c r="Q11" s="3">
         <v>1.17E-2</v>
       </c>
-      <c r="R11" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S11" s="7">
+      <c r="R11" s="3">
+        <v>2.212E-3</v>
+      </c>
+      <c r="S11" s="5">
         <v>1E-3</v>
       </c>
     </row>
@@ -9019,7 +9148,7 @@
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>1E-3</v>
       </c>
       <c r="C12" s="3">
@@ -9037,8 +9166,8 @@
       <c r="G12" s="3">
         <v>8.7131999999999997E-4</v>
       </c>
-      <c r="H12" s="7">
-        <v>1E-3</v>
+      <c r="H12" s="3">
+        <v>8.989E-4</v>
       </c>
       <c r="I12" s="3">
         <v>1.2378999999999999E-3</v>
@@ -9046,31 +9175,31 @@
       <c r="J12" s="3">
         <v>5.5035999999999996E-4</v>
       </c>
-      <c r="K12" s="7">
-        <v>1E-3</v>
+      <c r="K12" s="3">
+        <v>1.3142E-3</v>
       </c>
       <c r="L12" s="3">
         <v>1.8228000000000001E-3</v>
       </c>
-      <c r="M12" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="N12" s="7">
-        <v>5.3713000000000003E-4</v>
-      </c>
-      <c r="O12" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="P12" s="7">
+      <c r="M12" s="3">
+        <v>4.7538000000000002E-4</v>
+      </c>
+      <c r="N12" s="8">
+        <v>5.4595999999999996E-4</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1.2882E-3</v>
+      </c>
+      <c r="P12" s="5">
         <v>1E-3</v>
       </c>
       <c r="Q12" s="3">
         <v>9.4693999999999995E-6</v>
       </c>
-      <c r="R12" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S12" s="7">
+      <c r="R12" s="3">
+        <v>1.1594000000000001E-3</v>
+      </c>
+      <c r="S12" s="5">
         <v>1E-3</v>
       </c>
       <c r="U12" s="3"/>

</xml_diff>

<commit_message>
completed meanRates for all proteins and species
</commit_message>
<xml_diff>
--- a/20 Results/meanRate.xlsx
+++ b/20 Results/meanRate.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RVA" sheetId="4" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,18 +90,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -124,7 +118,6 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -146,7 +139,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -190,7 +183,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -322,6 +314,9 @@
                 <c:pt idx="4">
                   <c:v>1.8167000000000001E-3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3085E-3</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>2.6738E-3</c:v>
                 </c:pt>
@@ -341,7 +336,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -445,6 +440,9 @@
                 <c:pt idx="4">
                   <c:v>1.173E-3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8604999999999999E-4</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1.9653000000000001E-3</c:v>
                 </c:pt>
@@ -464,7 +462,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -568,6 +566,9 @@
                 <c:pt idx="4">
                   <c:v>5.5836000000000004E-4</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7810000000000001E-4</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>1.2939E-3</c:v>
                 </c:pt>
@@ -587,7 +588,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -651,7 +652,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -788,7 +788,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -905,7 +904,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -949,7 +948,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1103,7 +1101,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -1229,7 +1227,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -1355,7 +1353,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -1419,7 +1417,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1556,7 +1553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1673,7 +1669,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1717,7 +1713,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1861,11 +1856,17 @@
                 <c:pt idx="8">
                   <c:v>1.1016000000000001E-3</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8976000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8376999999999999E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0833-4893-9D63-15B54EF98E4E}"/>
             </c:ext>
@@ -1981,11 +1982,17 @@
                 <c:pt idx="8">
                   <c:v>7.8620000000000003E-4</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3479E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.4272E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0833-4893-9D63-15B54EF98E4E}"/>
             </c:ext>
@@ -2101,11 +2108,17 @@
                 <c:pt idx="8">
                   <c:v>4.7538000000000002E-4</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8549E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0653999999999998E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0833-4893-9D63-15B54EF98E4E}"/>
             </c:ext>
@@ -2169,7 +2182,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2306,7 +2318,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2423,7 +2434,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2467,7 +2478,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2615,7 +2625,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -2675,6 +2685,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2694,6 +2709,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2713,6 +2733,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2732,6 +2757,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2751,6 +2781,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2770,6 +2805,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2789,6 +2829,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2808,6 +2853,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2827,6 +2877,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -2846,6 +2901,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -2865,6 +2925,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -2884,6 +2949,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -2903,6 +2973,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -2922,6 +2997,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -2941,6 +3021,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-1CF6-4CFF-90B7-D4960B02297A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3020,7 +3105,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -3140,7 +3225,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -3218,7 +3303,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3355,7 +3439,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3472,7 +3555,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3516,7 +3599,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3619,7 +3701,7 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.3085E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.9718000000000002E-3</c:v>
@@ -3661,7 +3743,7 @@
                   <c:v>3.3138E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.8976000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2.7199999999999998E-2</c:v>
@@ -3670,13 +3752,13 @@
                   <c:v>3.3947000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.8376999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -3736,6 +3818,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3755,6 +3842,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3774,6 +3866,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3793,6 +3890,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3812,6 +3914,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3831,6 +3938,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3850,6 +3962,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -3869,6 +3986,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3888,6 +4010,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3907,6 +4034,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -3926,6 +4058,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -3945,6 +4082,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -3964,6 +4106,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -3983,6 +4130,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -4002,6 +4154,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -4021,6 +4178,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -4040,6 +4202,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -4059,6 +4226,11 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-EA1A-4093-80EC-E4C6B26B161D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4093,7 +4265,7 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>8.8604999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.5509999999999999E-3</c:v>
@@ -4135,7 +4307,7 @@
                   <c:v>2.2620000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.3479E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.17E-2</c:v>
@@ -4144,13 +4316,13 @@
                   <c:v>2.212E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.4272E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -4225,7 +4397,7 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>5.7810000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.6161000000000001E-3</c:v>
@@ -4267,7 +4439,7 @@
                   <c:v>1.2882E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.8549E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>9.4693999999999995E-6</c:v>
@@ -4276,13 +4448,13 @@
                   <c:v>1.1594000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1E-3</c:v>
+                  <c:v>2.0653999999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0BED-4C21-9D24-DC5C1D8052A6}"/>
             </c:ext>
@@ -4360,7 +4532,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4497,7 +4668,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7875,13 +8045,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7957,7 +8128,7 @@
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L9" t="s">
@@ -7983,7 +8154,9 @@
       <c r="F10" s="4">
         <v>1.8167000000000001E-3</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4">
+        <v>1.3085E-3</v>
+      </c>
       <c r="H10" s="4">
         <v>2.6738E-3</v>
       </c>
@@ -7993,7 +8166,7 @@
       <c r="J10" s="4">
         <v>3.4900999999999999E-3</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>1.9476000000000001E-3</v>
       </c>
       <c r="L10" s="4">
@@ -8019,6 +8192,9 @@
       <c r="F11" s="3">
         <v>1.173E-3</v>
       </c>
+      <c r="G11" s="4">
+        <v>8.8604999999999999E-4</v>
+      </c>
       <c r="H11" s="3">
         <v>1.9653000000000001E-3</v>
       </c>
@@ -8028,7 +8204,7 @@
       <c r="J11" s="3">
         <v>2.317E-3</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <v>1.1980000000000001E-3</v>
       </c>
       <c r="L11" s="3">
@@ -8054,7 +8230,9 @@
       <c r="F12" s="3">
         <v>5.5836000000000004E-4</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>5.7810000000000001E-4</v>
+      </c>
       <c r="H12" s="3">
         <v>1.2939E-3</v>
       </c>
@@ -8064,7 +8242,7 @@
       <c r="J12" s="3">
         <v>1.3142E-3</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>5.4595999999999996E-4</v>
       </c>
       <c r="L12" s="3">
@@ -8085,6 +8263,9 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
+      <c r="G14">
+        <v>706370000</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -8105,7 +8286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -8342,13 +8523,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8462,8 +8644,12 @@
       <c r="J10" s="4">
         <v>1.1016000000000001E-3</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="K10" s="4">
+        <v>2.8976000000000002E-3</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.8376999999999999E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -8496,6 +8682,12 @@
       <c r="J11" s="3">
         <v>7.8620000000000003E-4</v>
       </c>
+      <c r="K11" s="3">
+        <v>2.3479E-3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2.4272E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -8527,6 +8719,12 @@
       </c>
       <c r="J12" s="3">
         <v>4.7538000000000002E-4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.8549E-3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>2.0653999999999998E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -8535,6 +8733,12 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
+      <c r="K13">
+        <v>967100000</v>
+      </c>
+      <c r="L13">
+        <v>682520000</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -8906,8 +9110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:V15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9028,8 +9232,8 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
-        <v>1E-3</v>
+      <c r="B10" s="4">
+        <v>1.3085E-3</v>
       </c>
       <c r="C10" s="4">
         <v>3.9718000000000002E-3</v>
@@ -9064,14 +9268,14 @@
       <c r="M10" s="4">
         <v>1.1016000000000001E-3</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <v>1.9476000000000001E-3</v>
       </c>
       <c r="O10" s="4">
         <v>3.3138E-3</v>
       </c>
-      <c r="P10" s="5">
-        <v>1E-3</v>
+      <c r="P10" s="4">
+        <v>2.8976000000000002E-3</v>
       </c>
       <c r="Q10" s="4">
         <v>2.7199999999999998E-2</v>
@@ -9079,8 +9283,8 @@
       <c r="R10" s="4">
         <v>3.3947000000000001E-3</v>
       </c>
-      <c r="S10" s="5">
-        <v>1E-3</v>
+      <c r="S10" s="4">
+        <v>2.8376999999999999E-3</v>
       </c>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -9089,8 +9293,8 @@
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5">
-        <v>1E-3</v>
+      <c r="B11" s="4">
+        <v>8.8604999999999999E-4</v>
       </c>
       <c r="C11" s="3">
         <v>2.5509999999999999E-3</v>
@@ -9125,14 +9329,14 @@
       <c r="M11" s="3">
         <v>7.8620000000000003E-4</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <v>1.1980000000000001E-3</v>
       </c>
       <c r="O11" s="3">
         <v>2.2620000000000001E-3</v>
       </c>
-      <c r="P11" s="5">
-        <v>1E-3</v>
+      <c r="P11" s="3">
+        <v>2.3479E-3</v>
       </c>
       <c r="Q11" s="3">
         <v>1.17E-2</v>
@@ -9140,16 +9344,16 @@
       <c r="R11" s="3">
         <v>2.212E-3</v>
       </c>
-      <c r="S11" s="5">
-        <v>1E-3</v>
+      <c r="S11" s="3">
+        <v>2.4272E-3</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
-        <v>1E-3</v>
+      <c r="B12" s="3">
+        <v>5.7810000000000001E-4</v>
       </c>
       <c r="C12" s="3">
         <v>1.6161000000000001E-3</v>
@@ -9184,14 +9388,14 @@
       <c r="M12" s="3">
         <v>4.7538000000000002E-4</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <v>5.4595999999999996E-4</v>
       </c>
       <c r="O12" s="3">
         <v>1.2882E-3</v>
       </c>
-      <c r="P12" s="5">
-        <v>1E-3</v>
+      <c r="P12" s="3">
+        <v>1.8549E-3</v>
       </c>
       <c r="Q12" s="3">
         <v>9.4693999999999995E-6</v>
@@ -9199,8 +9403,8 @@
       <c r="R12" s="3">
         <v>1.1594000000000001E-3</v>
       </c>
-      <c r="S12" s="5">
-        <v>1E-3</v>
+      <c r="S12" s="3">
+        <v>2.0653999999999998E-3</v>
       </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>

</xml_diff>

<commit_message>
changes to data table
</commit_message>
<xml_diff>
--- a/20 Results/meanRate.xlsx
+++ b/20 Results/meanRate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="23">
   <si>
     <t>NSP1</t>
   </si>
@@ -93,11 +93,17 @@
   <si>
     <t>Table 6: Evolutionary Rates over Time of Different RV Genes (Substitutions/Site/Year)</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,49 +234,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10670,208 +10679,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:R13"/>
+  <dimension ref="C4:R14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
     </row>
     <row r="5" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="O6" s="29"/>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="3:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="16">
         <v>3.8528E-3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="16">
         <v>7.1290999999999998E-4</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="15">
         <v>1.9436E-3</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="15">
         <v>1.5365000000000001E-3</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="15">
         <v>1.173E-3</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="17">
         <v>8.8604999999999999E-4</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="15">
         <v>1.9653000000000001E-3</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="15">
         <v>1.421E-3</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="15">
         <v>2.317E-3</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="18">
         <v>1.1980000000000001E-3</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="15">
         <v>1.17E-2</v>
       </c>
-      <c r="P7" s="3">
+      <c r="O7" s="19">
         <f>AVERAGE(D7:N7)</f>
         <v>2.6096509090909091E-3</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="20">
         <f>AVERAGE(D7:H9)</f>
         <v>9.9787606666666695E-3</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+    <row r="8" spans="3:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="16">
         <v>4.539E-2</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="16">
         <v>1.8240000000000001E-3</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="15">
         <v>2.8046999999999998E-3</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="15">
         <v>4.4450000000000003E-2</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="15">
         <v>2.23E-2</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="15">
         <v>2.5509999999999999E-3</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="15">
         <v>8.7130000000000003E-3</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="15">
         <v>2.9180000000000001E-2</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="15">
         <v>2.9099999999999998E-3</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="15">
         <v>2.2620000000000001E-3</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="15">
         <v>2.212E-3</v>
       </c>
-      <c r="P8" s="3">
-        <f t="shared" ref="P8:P9" si="0">AVERAGE(D8:N8)</f>
+      <c r="O8" s="19">
+        <f>AVERAGE(D8:N8)</f>
         <v>1.4963336363636363E-2</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="20">
         <f>AVERAGE(I7:N9)</f>
         <v>4.3462583333333344E-3</v>
       </c>
     </row>
-    <row r="9" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="17" t="s">
+    <row r="9" spans="3:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>4.398E-3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <v>5.329E-4</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <v>1.6969999999999999E-3</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="15">
         <v>1.601E-2</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="15">
         <v>1.0560000000000001E-3</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="15">
         <v>1.263E-3</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="15">
         <v>2.4729999999999999E-3</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="15">
         <v>1.6199999999999999E-3</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="15">
         <v>7.8620000000000003E-4</v>
       </c>
       <c r="M9" s="21">
@@ -10880,79 +10895,123 @@
       <c r="N9" s="21">
         <v>2.4272E-3</v>
       </c>
-      <c r="P9" s="3">
+      <c r="O9" s="19">
+        <f>AVERAGE(D9:N9)</f>
+        <v>3.1464727272727273E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="23">
+        <v>1.7880266666666669E-2</v>
+      </c>
+      <c r="E10" s="23">
+        <v>1.02327E-3</v>
+      </c>
+      <c r="F10" s="23">
+        <v>2.1484333333333331E-3</v>
+      </c>
+      <c r="G10" s="23">
+        <v>2.0665500000000003E-2</v>
+      </c>
+      <c r="H10" s="23">
+        <v>8.1763333333333341E-3</v>
+      </c>
+      <c r="I10" s="23">
+        <v>1.5666833333333333E-3</v>
+      </c>
+      <c r="J10" s="23">
+        <v>4.3837666666666662E-3</v>
+      </c>
+      <c r="K10" s="23">
+        <v>1.0740333333333333E-2</v>
+      </c>
+      <c r="L10" s="23">
+        <v>2.0043999999999999E-3</v>
+      </c>
+      <c r="M10" s="23">
+        <v>1.9359666666666669E-3</v>
+      </c>
+      <c r="N10" s="23">
+        <v>5.4464000000000005E-3</v>
+      </c>
+      <c r="O10" s="23">
+        <f>AVERAGE(O7:O9,D10:N10)</f>
+        <v>6.9064866666666679E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D14" s="13">
+        <f t="shared" ref="D14:N14" si="0">AVERAGE(D7:D9)</f>
+        <v>1.7880266666666669E-2</v>
+      </c>
+      <c r="E14" s="14">
         <f t="shared" si="0"/>
-        <v>3.1464727272727273E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="3:18" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D13" s="25">
-        <f>AVERAGE(D7:D9)</f>
-        <v>1.7880266666666669E-2</v>
-      </c>
-      <c r="E13" s="26">
-        <f t="shared" ref="E13:N13" si="1">AVERAGE(E7:E9)</f>
         <v>1.02327E-3</v>
       </c>
-      <c r="F13" s="23">
-        <f t="shared" si="1"/>
+      <c r="F14" s="11">
+        <f t="shared" si="0"/>
         <v>2.1484333333333331E-3</v>
       </c>
-      <c r="G13" s="25">
-        <f t="shared" si="1"/>
+      <c r="G14" s="13">
+        <f t="shared" si="0"/>
         <v>2.0665500000000003E-2</v>
       </c>
-      <c r="H13" s="23">
-        <f t="shared" si="1"/>
+      <c r="H14" s="11">
+        <f t="shared" si="0"/>
         <v>8.1763333333333341E-3</v>
       </c>
-      <c r="I13" s="26">
-        <f t="shared" si="1"/>
+      <c r="I14" s="14">
+        <f t="shared" si="0"/>
         <v>1.5666833333333333E-3</v>
       </c>
-      <c r="J13" s="24">
-        <f t="shared" si="1"/>
+      <c r="J14" s="12">
+        <f t="shared" si="0"/>
         <v>4.3837666666666662E-3</v>
       </c>
-      <c r="K13" s="25">
-        <f t="shared" si="1"/>
+      <c r="K14" s="13">
+        <f t="shared" si="0"/>
         <v>1.0740333333333333E-2</v>
       </c>
-      <c r="L13" s="24">
-        <f t="shared" si="1"/>
+      <c r="L14" s="12">
+        <f t="shared" si="0"/>
         <v>2.0043999999999999E-3</v>
       </c>
-      <c r="M13" s="26">
-        <f t="shared" si="1"/>
+      <c r="M14" s="14">
+        <f t="shared" si="0"/>
         <v>1.9359666666666669E-3</v>
       </c>
-      <c r="N13" s="24">
-        <f t="shared" si="1"/>
+      <c r="N14" s="12">
+        <f t="shared" si="0"/>
         <v>5.4464000000000005E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D5:N5"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:O11"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="O5:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10963,7 +11022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -11441,8 +11500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:L11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>